<commit_message>
cpsat-hoz file ellenőrzés hozzáírva, kommentek átírva
</commit_message>
<xml_diff>
--- a/cpsat_solver/requests_admin_cp.xlsx
+++ b/cpsat_solver/requests_admin_cp.xlsx
@@ -657,7 +657,7 @@
   <dimension ref="A1:AQ12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -790,7 +790,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="10"/>

</xml_diff>